<commit_message>
Added requests and request summaries
</commit_message>
<xml_diff>
--- a/FlockAuditLogs/EPDLocalFlockSearchAudit_ConsecutiveDayAnomalies_2025-09-22.xlsx
+++ b/FlockAuditLogs/EPDLocalFlockSearchAudit_ConsecutiveDayAnomalies_2025-09-22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoecs-my.sharepoint.com/personal/sethm_uoecs_org/Documents/Personal/EOE/repos/eugene-oregon/FlockAuditLogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{0C6F1F5A-4598-4E23-8821-48C8DA895981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97AAC0F2-8AC7-4654-BD68-7B6D2115F779}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{0C6F1F5A-4598-4E23-8821-48C8DA895981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04CE4302-EF66-4DD6-A151-17E3BBEB22E9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="737" xr2:uid="{38FCAACE-6C1F-4684-9057-6927D9BBE020}"/>
+    <workbookView xWindow="-57697" yWindow="-8160" windowWidth="28995" windowHeight="15675" tabRatio="737" activeTab="5" xr2:uid="{38FCAACE-6C1F-4684-9057-6927D9BBE020}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="7" r:id="rId1"/>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>Event 2</t>
-  </si>
-  <si>
-    <t>1 person, 36 searches, 9 consecutive days</t>
   </si>
   <si>
     <t>Event 3</t>
@@ -1591,6 +1588,9 @@
   </si>
   <si>
     <t>Consecutive Search Day Analysis</t>
+  </si>
+  <si>
+    <t>1 person, 27 searches, 9 consecutive days</t>
   </si>
 </sst>
 </file>
@@ -1952,6 +1952,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2383,81 +2387,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079E71F2-07B4-40D1-A1BF-F2BB37156FC0}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.85546875" customWidth="1"/>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A1" s="9" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="24" x14ac:dyDescent="0.4">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="16" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="24" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="13" spans="1:1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="15" spans="1:1" ht="231.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>484</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="231.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -2478,30 +2482,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -2512,18 +2516,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5">
         <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>54</v>
       </c>
@@ -2534,73 +2538,73 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7">
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8">
         <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9">
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B10">
         <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11">
         <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12">
         <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>14575771</v>
       </c>
@@ -2608,219 +2612,219 @@
         <v>68</v>
       </c>
       <c r="C13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>227</v>
       </c>
       <c r="B14">
         <v>66</v>
       </c>
       <c r="C14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>229</v>
       </c>
       <c r="B15">
         <v>66</v>
       </c>
       <c r="C15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>231</v>
       </c>
       <c r="B16">
         <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B17">
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B18">
         <v>61</v>
       </c>
       <c r="C18" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>235</v>
       </c>
       <c r="B19">
         <v>60</v>
       </c>
       <c r="C19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>237</v>
       </c>
       <c r="B20">
         <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B21">
         <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B22">
         <v>54</v>
       </c>
       <c r="C22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>241</v>
       </c>
       <c r="B23">
         <v>54</v>
       </c>
       <c r="C23" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>243</v>
       </c>
       <c r="B24">
         <v>47</v>
       </c>
       <c r="C24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>245</v>
       </c>
       <c r="B25">
         <v>42</v>
       </c>
       <c r="C25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>247</v>
       </c>
       <c r="B26">
         <v>41</v>
       </c>
       <c r="C26" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>249</v>
       </c>
       <c r="B27">
         <v>41</v>
       </c>
       <c r="C27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>251</v>
       </c>
       <c r="B28">
         <v>40</v>
       </c>
       <c r="C28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>253</v>
       </c>
       <c r="B29">
         <v>40</v>
       </c>
       <c r="C29" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>255</v>
       </c>
       <c r="B30">
         <v>40</v>
       </c>
       <c r="C30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>257</v>
       </c>
       <c r="B31">
         <v>38</v>
       </c>
       <c r="C31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>259</v>
       </c>
       <c r="B32">
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>46532411</v>
       </c>
@@ -2828,692 +2832,692 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>262</v>
       </c>
       <c r="B34">
         <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>264</v>
       </c>
       <c r="B35">
         <v>37</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>266</v>
       </c>
       <c r="B36">
         <v>37</v>
       </c>
       <c r="C36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>268</v>
       </c>
       <c r="B37">
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B38">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B39">
         <v>35</v>
       </c>
       <c r="C39" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>272</v>
       </c>
       <c r="B40">
         <v>35</v>
       </c>
       <c r="C40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>274</v>
       </c>
       <c r="B41">
         <v>33</v>
       </c>
       <c r="C41" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>276</v>
       </c>
       <c r="B42">
         <v>33</v>
       </c>
       <c r="C42" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>278</v>
       </c>
       <c r="B43">
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>280</v>
       </c>
       <c r="B44">
         <v>32</v>
       </c>
       <c r="C44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>282</v>
       </c>
       <c r="B45">
         <v>31</v>
       </c>
       <c r="C45" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>284</v>
       </c>
       <c r="B46">
         <v>30</v>
       </c>
       <c r="C46" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>286</v>
       </c>
       <c r="B47">
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B48">
         <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B49">
         <v>27</v>
       </c>
       <c r="C49" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>290</v>
       </c>
       <c r="B50">
         <v>27</v>
       </c>
       <c r="C50" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>292</v>
       </c>
       <c r="B51">
         <v>25</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="13" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>294</v>
       </c>
       <c r="B52">
         <v>24</v>
       </c>
       <c r="C52" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>296</v>
       </c>
       <c r="B53">
         <v>23</v>
       </c>
       <c r="C53" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
-        <v>298</v>
       </c>
       <c r="B54">
         <v>22</v>
       </c>
       <c r="C54" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
-        <v>300</v>
       </c>
       <c r="B55">
         <v>22</v>
       </c>
       <c r="C55" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
-        <v>302</v>
       </c>
       <c r="B56">
         <v>21</v>
       </c>
       <c r="C56" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>304</v>
       </c>
       <c r="B57">
         <v>21</v>
       </c>
       <c r="C57" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
         <v>305</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>306</v>
       </c>
       <c r="B58">
         <v>21</v>
       </c>
       <c r="C58" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
-        <v>308</v>
       </c>
       <c r="B59">
         <v>20</v>
       </c>
       <c r="C59" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
-        <v>310</v>
       </c>
       <c r="B60">
         <v>20</v>
       </c>
       <c r="C60" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>312</v>
       </c>
       <c r="B61">
         <v>19</v>
       </c>
       <c r="C61" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="13" t="s">
         <v>313</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
-        <v>314</v>
       </c>
       <c r="B62">
         <v>19</v>
       </c>
       <c r="C62" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
         <v>315</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>316</v>
       </c>
       <c r="B63">
         <v>19</v>
       </c>
       <c r="C63" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
-        <v>318</v>
       </c>
       <c r="B64">
         <v>19</v>
       </c>
       <c r="C64" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>320</v>
       </c>
       <c r="B65">
         <v>18</v>
       </c>
       <c r="C65" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
-        <v>322</v>
       </c>
       <c r="B66">
         <v>18</v>
       </c>
       <c r="C66" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>324</v>
       </c>
       <c r="B67">
         <v>17</v>
       </c>
       <c r="C67" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>326</v>
       </c>
       <c r="B68">
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B69">
         <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B70">
         <v>16</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="13" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
-        <v>330</v>
       </c>
       <c r="B71">
         <v>15</v>
       </c>
       <c r="C71" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="13" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>332</v>
       </c>
       <c r="B72">
         <v>15</v>
       </c>
       <c r="C72" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="13" t="s">
         <v>333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
-        <v>334</v>
       </c>
       <c r="B73">
         <v>15</v>
       </c>
       <c r="C73" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
-        <v>336</v>
       </c>
       <c r="B74">
         <v>15</v>
       </c>
       <c r="C74" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="13" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
-        <v>338</v>
       </c>
       <c r="B75">
         <v>15</v>
       </c>
       <c r="C75" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
-        <v>340</v>
       </c>
       <c r="B76">
         <v>15</v>
       </c>
       <c r="C76" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="13" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
-        <v>342</v>
       </c>
       <c r="B77">
         <v>13</v>
       </c>
       <c r="C77" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="13" t="s">
         <v>343</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
-        <v>344</v>
       </c>
       <c r="B78">
         <v>13</v>
       </c>
       <c r="C78" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="13" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>346</v>
       </c>
       <c r="B79">
         <v>13</v>
       </c>
       <c r="C79" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="13" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>348</v>
       </c>
       <c r="B80">
         <v>12</v>
       </c>
       <c r="C80" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="13" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
-        <v>350</v>
       </c>
       <c r="B81">
         <v>12</v>
       </c>
       <c r="C81" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="13" t="s">
         <v>351</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
-        <v>352</v>
       </c>
       <c r="B82">
         <v>11</v>
       </c>
       <c r="C82" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="13" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
-        <v>354</v>
       </c>
       <c r="B83">
         <v>11</v>
       </c>
       <c r="C83" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="13" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
-        <v>356</v>
       </c>
       <c r="B84">
         <v>11</v>
       </c>
       <c r="C84" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="13" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>358</v>
       </c>
       <c r="B85">
         <v>11</v>
       </c>
       <c r="C85" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="13" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>360</v>
       </c>
       <c r="B86">
         <v>11</v>
       </c>
       <c r="C86" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="13" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>362</v>
       </c>
       <c r="B87">
         <v>10</v>
       </c>
       <c r="C87" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="13" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>364</v>
       </c>
       <c r="B88">
         <v>10</v>
       </c>
       <c r="C88" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="13" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
-        <v>366</v>
       </c>
       <c r="B89">
         <v>10</v>
       </c>
       <c r="C89" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="13" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
-        <v>368</v>
       </c>
       <c r="B90">
         <v>10</v>
       </c>
       <c r="C90" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="13" t="s">
         <v>369</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="s">
-        <v>370</v>
       </c>
       <c r="B91">
         <v>10</v>
       </c>
       <c r="C91" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="13" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
-        <v>372</v>
       </c>
       <c r="B92">
         <v>10</v>
       </c>
       <c r="C92" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="13" t="s">
         <v>373</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="B93">
         <v>10</v>
       </c>
       <c r="C93" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
         <v>375</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
-        <v>376</v>
       </c>
       <c r="B94">
         <v>10</v>
       </c>
       <c r="C94" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="13" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="13" t="s">
-        <v>378</v>
       </c>
       <c r="B95">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="13">
         <v>23739276</v>
       </c>
@@ -3521,546 +3525,546 @@
         <v>9</v>
       </c>
       <c r="C96" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="13" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="13" t="s">
-        <v>381</v>
       </c>
       <c r="B97">
         <v>8</v>
       </c>
       <c r="C97" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="13" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="13" t="s">
-        <v>383</v>
       </c>
       <c r="B98">
         <v>8</v>
       </c>
       <c r="C98" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="13" t="s">
-        <v>385</v>
       </c>
       <c r="B99">
         <v>7</v>
       </c>
       <c r="C99" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="13" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
-        <v>387</v>
       </c>
       <c r="B100">
         <v>7</v>
       </c>
       <c r="C100" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="13" t="s">
         <v>388</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
-        <v>389</v>
       </c>
       <c r="B101">
         <v>7</v>
       </c>
       <c r="C101" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="13" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
-        <v>391</v>
       </c>
       <c r="B102">
         <v>7</v>
       </c>
       <c r="C102" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="13" t="s">
         <v>392</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="s">
-        <v>393</v>
       </c>
       <c r="B103">
         <v>7</v>
       </c>
       <c r="C103" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="13" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
-        <v>395</v>
       </c>
       <c r="B104">
         <v>7</v>
       </c>
       <c r="C104" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="14" t="s">
         <v>396</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="s">
-        <v>397</v>
       </c>
       <c r="B105">
         <v>7</v>
       </c>
       <c r="C105" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="13" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="s">
-        <v>399</v>
       </c>
       <c r="B106">
         <v>6</v>
       </c>
       <c r="C106" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="13" t="s">
         <v>400</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
-        <v>401</v>
       </c>
       <c r="B107">
         <v>6</v>
       </c>
       <c r="C107" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="13" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
-        <v>403</v>
       </c>
       <c r="B108">
         <v>5</v>
       </c>
       <c r="C108" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="13" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="s">
-        <v>405</v>
       </c>
       <c r="B109">
         <v>5</v>
       </c>
       <c r="C109" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="13" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="13" t="s">
-        <v>407</v>
       </c>
       <c r="B110">
         <v>5</v>
       </c>
       <c r="C110" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="13" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="13" t="s">
-        <v>409</v>
       </c>
       <c r="B111">
         <v>5</v>
       </c>
       <c r="C111" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="13" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="s">
-        <v>411</v>
       </c>
       <c r="B112">
         <v>5</v>
       </c>
       <c r="C112" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="13" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="B113">
         <v>4</v>
       </c>
       <c r="C113" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="13" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
-        <v>415</v>
       </c>
       <c r="B114">
         <v>4</v>
       </c>
       <c r="C114" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="13" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="13" t="s">
-        <v>417</v>
       </c>
       <c r="B115">
         <v>4</v>
       </c>
       <c r="C115" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="13" t="s">
         <v>418</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="s">
-        <v>419</v>
       </c>
       <c r="B116">
         <v>4</v>
       </c>
       <c r="C116" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="13" t="s">
         <v>420</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="13" t="s">
-        <v>421</v>
       </c>
       <c r="B117">
         <v>4</v>
       </c>
       <c r="C117" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="13" t="s">
         <v>422</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="13" t="s">
-        <v>423</v>
       </c>
       <c r="B118">
         <v>3</v>
       </c>
       <c r="C118" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="13" t="s">
         <v>424</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
-        <v>425</v>
       </c>
       <c r="B119">
         <v>3</v>
       </c>
       <c r="C119" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="13" t="s">
         <v>426</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="13" t="s">
-        <v>427</v>
       </c>
       <c r="B120">
         <v>3</v>
       </c>
       <c r="C120" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="13" t="s">
         <v>428</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="s">
-        <v>429</v>
       </c>
       <c r="B121">
         <v>3</v>
       </c>
       <c r="C121" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="13" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="s">
-        <v>431</v>
       </c>
       <c r="B122">
         <v>3</v>
       </c>
       <c r="C122" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="13" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="13" t="s">
-        <v>433</v>
       </c>
       <c r="B123">
         <v>3</v>
       </c>
       <c r="C123" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="13" t="s">
         <v>434</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="13" t="s">
-        <v>435</v>
       </c>
       <c r="B124">
         <v>3</v>
       </c>
       <c r="C124" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="13" t="s">
         <v>436</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="13" t="s">
-        <v>437</v>
       </c>
       <c r="B125">
         <v>3</v>
       </c>
       <c r="C125" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="13" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="13" t="s">
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
         <v>439</v>
       </c>
-      <c r="B126">
-        <v>2</v>
-      </c>
-      <c r="C126" t="s">
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="13" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="13" t="s">
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
         <v>441</v>
       </c>
-      <c r="B127">
-        <v>2</v>
-      </c>
-      <c r="C127" t="s">
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="13" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="13" t="s">
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128" t="s">
         <v>443</v>
       </c>
-      <c r="B128">
-        <v>2</v>
-      </c>
-      <c r="C128" t="s">
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="13" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="13" t="s">
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="C129" t="s">
         <v>445</v>
       </c>
-      <c r="B129">
-        <v>2</v>
-      </c>
-      <c r="C129" t="s">
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="13" t="s">
+      <c r="B130">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
         <v>447</v>
       </c>
-      <c r="B130">
-        <v>2</v>
-      </c>
-      <c r="C130" t="s">
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="13" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="13" t="s">
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
         <v>449</v>
       </c>
-      <c r="B131">
-        <v>2</v>
-      </c>
-      <c r="C131" t="s">
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="13" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="13" t="s">
+      <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
         <v>451</v>
       </c>
-      <c r="B132">
-        <v>2</v>
-      </c>
-      <c r="C132" t="s">
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="13" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
         <v>453</v>
       </c>
-      <c r="B133">
-        <v>2</v>
-      </c>
-      <c r="C133" t="s">
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="13" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="13" t="s">
+      <c r="B134">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
         <v>455</v>
       </c>
-      <c r="B134">
-        <v>2</v>
-      </c>
-      <c r="C134" t="s">
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="13" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="13" t="s">
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="C135" t="s">
         <v>457</v>
       </c>
-      <c r="B135">
-        <v>2</v>
-      </c>
-      <c r="C135" t="s">
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="13" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="13" t="s">
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
         <v>459</v>
       </c>
-      <c r="B136">
-        <v>1</v>
-      </c>
-      <c r="C136" t="s">
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="13" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="13" t="s">
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
         <v>461</v>
       </c>
-      <c r="B137">
-        <v>1</v>
-      </c>
-      <c r="C137" t="s">
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="13" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="13" t="s">
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
         <v>463</v>
       </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-      <c r="C138" t="s">
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="13" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="13" t="s">
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
         <v>465</v>
       </c>
-      <c r="B139">
-        <v>1</v>
-      </c>
-      <c r="C139" t="s">
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="13" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="13" t="s">
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
         <v>467</v>
       </c>
-      <c r="B140">
-        <v>1</v>
-      </c>
-      <c r="C140" t="s">
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="13" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="13" t="s">
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
         <v>469</v>
       </c>
-      <c r="B141">
-        <v>1</v>
-      </c>
-      <c r="C141" t="s">
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="13" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="13" t="s">
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
         <v>471</v>
       </c>
-      <c r="B142">
-        <v>1</v>
-      </c>
-      <c r="C142" t="s">
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="13" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="13" t="s">
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
         <v>473</v>
       </c>
-      <c r="B143">
-        <v>1</v>
-      </c>
-      <c r="C143" t="s">
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="13" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="13" t="s">
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
         <v>475</v>
       </c>
-      <c r="B144">
-        <v>1</v>
-      </c>
-      <c r="C144" t="s">
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="13" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="13" t="s">
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
         <v>477</v>
-      </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-      <c r="C145" t="s">
-        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4079,38 +4083,38 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
         <v>195</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>196</v>
-      </c>
-      <c r="D3" t="s">
-        <v>197</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4127,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -4144,7 +4148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -4161,9 +4165,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4175,10 +4179,10 @@
         <v>45881</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -4195,9 +4199,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -4209,12 +4213,12 @@
         <v>45885</v>
       </c>
       <c r="E9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -4226,12 +4230,12 @@
         <v>45886</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -4243,12 +4247,12 @@
         <v>45913</v>
       </c>
       <c r="E11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -4260,12 +4264,12 @@
         <v>45848</v>
       </c>
       <c r="E12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>202</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -4277,12 +4281,12 @@
         <v>45864</v>
       </c>
       <c r="E13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -4294,12 +4298,12 @@
         <v>45877</v>
       </c>
       <c r="E14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -4311,12 +4315,12 @@
         <v>45884</v>
       </c>
       <c r="E15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>204</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -4328,12 +4332,12 @@
         <v>45844</v>
       </c>
       <c r="E16" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -4345,12 +4349,12 @@
         <v>45872</v>
       </c>
       <c r="E17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>206</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -4362,12 +4366,12 @@
         <v>45891</v>
       </c>
       <c r="E18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>208</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -4379,10 +4383,10 @@
         <v>45878</v>
       </c>
       <c r="E19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -4399,7 +4403,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -4416,7 +4420,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -4433,9 +4437,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -4447,12 +4451,12 @@
         <v>45872</v>
       </c>
       <c r="E23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>212</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -4464,10 +4468,10 @@
         <v>45871</v>
       </c>
       <c r="E24" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -4484,7 +4488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4501,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -4518,9 +4522,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -4532,12 +4536,12 @@
         <v>45835</v>
       </c>
       <c r="E28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>176</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -4549,12 +4553,12 @@
         <v>45870</v>
       </c>
       <c r="E29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -4566,7 +4570,7 @@
         <v>45900</v>
       </c>
       <c r="E30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4581,30 +4585,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7392CB-A6D2-464F-B02D-3C8B35458658}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -4621,7 +4625,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4638,7 +4642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4655,7 +4659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4672,7 +4676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -4689,7 +4693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4706,7 +4710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4723,7 +4727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4740,7 +4744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4774,7 +4778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -4791,7 +4795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -4808,7 +4812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -4825,7 +4829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4842,7 +4846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -4859,7 +4863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -4876,7 +4880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -4893,7 +4897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -4910,7 +4914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -4927,7 +4931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -4944,7 +4948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -4961,7 +4965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -4978,7 +4982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -4995,7 +4999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -5012,7 +5016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -5029,7 +5033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -5046,7 +5050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -5063,7 +5067,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -5080,7 +5084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -5097,7 +5101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -5114,7 +5118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -5131,7 +5135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -5148,7 +5152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -5165,7 +5169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -5182,7 +5186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -5199,7 +5203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -5216,7 +5220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -5246,29 +5250,29 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -5285,7 +5289,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -5302,7 +5306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -5319,7 +5323,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -5336,7 +5340,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -5353,7 +5357,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -5370,7 +5374,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -5387,7 +5391,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -5404,7 +5408,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -5438,7 +5442,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -5455,7 +5459,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
@@ -5472,7 +5476,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -5489,7 +5493,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -5506,7 +5510,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -5523,7 +5527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>75</v>
       </c>
@@ -5540,7 +5544,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -5557,7 +5561,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -5574,7 +5578,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -5591,7 +5595,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -5608,7 +5612,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -5625,7 +5629,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -5642,7 +5646,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -5659,7 +5663,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -5676,7 +5680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -5693,7 +5697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -5710,7 +5714,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -5727,7 +5731,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -5756,30 +5760,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F31F70C-5188-44DA-969F-9135409F18CE}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -5796,7 +5800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -5813,7 +5817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -5830,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -5847,7 +5851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -5864,7 +5868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -5881,7 +5885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -5898,7 +5902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -5915,7 +5919,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -5932,7 +5936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -5949,7 +5953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -5966,7 +5970,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -5983,7 +5987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -6000,7 +6004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -6017,7 +6021,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -6034,7 +6038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -6051,7 +6055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -6068,7 +6072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>110</v>
       </c>
@@ -6085,7 +6089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -6102,7 +6106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -6119,7 +6123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -6136,7 +6140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -6153,7 +6157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -6170,7 +6174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -6187,7 +6191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -6204,7 +6208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -6221,7 +6225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -6254,26 +6258,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -6290,15 +6294,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
         <v>126</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
       </c>
       <c r="D4" s="1">
         <v>45876.842511574076</v>
@@ -6307,15 +6311,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
         <v>127</v>
-      </c>
-      <c r="C5" t="s">
-        <v>128</v>
       </c>
       <c r="D5" s="1">
         <v>45877.867893518516</v>
@@ -6324,15 +6328,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
         <v>127</v>
-      </c>
-      <c r="C6" t="s">
-        <v>128</v>
       </c>
       <c r="D6" s="1">
         <v>45877.886053240742</v>
@@ -6341,15 +6345,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
         <v>127</v>
-      </c>
-      <c r="C7" t="s">
-        <v>128</v>
       </c>
       <c r="D7" s="1">
         <v>45877.952615740738</v>
@@ -6358,15 +6362,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
         <v>127</v>
-      </c>
-      <c r="C8" t="s">
-        <v>128</v>
       </c>
       <c r="D8" s="1">
         <v>45878.78297453704</v>
@@ -6375,15 +6379,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
         <v>127</v>
-      </c>
-      <c r="C9" t="s">
-        <v>128</v>
       </c>
       <c r="D9" s="1">
         <v>45879.895648148151</v>
@@ -6392,15 +6396,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
         <v>127</v>
-      </c>
-      <c r="C10" t="s">
-        <v>128</v>
       </c>
       <c r="D10" s="1">
         <v>45879.948981481481</v>
@@ -6409,15 +6413,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
       </c>
       <c r="D11" s="1">
         <v>45880.907164351855</v>
@@ -6426,15 +6430,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
         <v>127</v>
-      </c>
-      <c r="C12" t="s">
-        <v>128</v>
       </c>
       <c r="D12" s="1">
         <v>45880.918553240743</v>
@@ -6443,15 +6447,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
         <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>128</v>
       </c>
       <c r="D13" s="1">
         <v>45881.607939814814</v>
@@ -6460,15 +6464,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
         <v>127</v>
-      </c>
-      <c r="C14" t="s">
-        <v>128</v>
       </c>
       <c r="D14" s="1">
         <v>45881.639039351852</v>
@@ -6477,15 +6481,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
         <v>127</v>
-      </c>
-      <c r="C15" t="s">
-        <v>128</v>
       </c>
       <c r="D15" s="1">
         <v>45881.850891203707</v>
@@ -6510,26 +6514,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -6546,9 +6550,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -6563,9 +6567,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -6577,12 +6581,12 @@
         <v>45852.388715277775</v>
       </c>
       <c r="E5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>147</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -6594,12 +6598,12 @@
         <v>45852.48028935185</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -6614,9 +6618,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -6628,12 +6632,12 @@
         <v>45852.527708333335</v>
       </c>
       <c r="E8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -6645,12 +6649,12 @@
         <v>45852.606782407405</v>
       </c>
       <c r="E9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -6662,12 +6666,12 @@
         <v>45852.632916666669</v>
       </c>
       <c r="E10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>154</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -6679,12 +6683,12 @@
         <v>45852.635740740741</v>
       </c>
       <c r="E11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>156</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -6696,12 +6700,12 @@
         <v>45852.640787037039</v>
       </c>
       <c r="E12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -6716,9 +6720,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -6730,12 +6734,12 @@
         <v>45852.695324074077</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -6750,9 +6754,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -6764,12 +6768,12 @@
         <v>45853.392974537041</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -6784,9 +6788,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -6801,9 +6805,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -6815,12 +6819,12 @@
         <v>45854.277442129627</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -6835,9 +6839,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -6849,12 +6853,12 @@
         <v>45854.428553240738</v>
       </c>
       <c r="E21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -6866,12 +6870,12 @@
         <v>45854.460798611108</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -6886,9 +6890,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -6903,9 +6907,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -6920,9 +6924,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -6937,9 +6941,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -6970,29 +6974,29 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
         <v>193</v>
       </c>
-      <c r="B2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -7009,15 +7013,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
         <v>174</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>175</v>
-      </c>
-      <c r="C4" t="s">
-        <v>176</v>
       </c>
       <c r="D4" s="1">
         <v>45880.467326388891</v>
@@ -7026,15 +7030,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="s">
         <v>175</v>
-      </c>
-      <c r="C5" t="s">
-        <v>176</v>
       </c>
       <c r="D5" s="1">
         <v>45880.469340277778</v>
@@ -7043,15 +7047,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
         <v>175</v>
-      </c>
-      <c r="C6" t="s">
-        <v>176</v>
       </c>
       <c r="D6" s="1">
         <v>45881.654328703706</v>
@@ -7060,15 +7064,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
         <v>175</v>
-      </c>
-      <c r="C7" t="s">
-        <v>176</v>
       </c>
       <c r="D7" s="1">
         <v>45881.850798611114</v>
@@ -7077,15 +7081,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" t="s">
         <v>175</v>
-      </c>
-      <c r="C8" t="s">
-        <v>176</v>
       </c>
       <c r="D8" s="1">
         <v>45882.342986111114</v>
@@ -7094,15 +7098,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" t="s">
         <v>175</v>
-      </c>
-      <c r="C9" t="s">
-        <v>176</v>
       </c>
       <c r="D9" s="1">
         <v>45883.453587962962</v>
@@ -7111,15 +7115,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
         <v>175</v>
-      </c>
-      <c r="C10" t="s">
-        <v>176</v>
       </c>
       <c r="D10" s="1">
         <v>45883.460451388892</v>
@@ -7128,15 +7132,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" t="s">
         <v>175</v>
-      </c>
-      <c r="C11" t="s">
-        <v>176</v>
       </c>
       <c r="D11" s="1">
         <v>45883.465925925928</v>
@@ -7145,15 +7149,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" t="s">
         <v>175</v>
-      </c>
-      <c r="C12" t="s">
-        <v>176</v>
       </c>
       <c r="D12" s="1">
         <v>45884.679479166669</v>
@@ -7162,15 +7166,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" t="s">
         <v>175</v>
-      </c>
-      <c r="C13" t="s">
-        <v>176</v>
       </c>
       <c r="D13" s="1">
         <v>45885.426990740743</v>
@@ -7179,15 +7183,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" t="s">
         <v>175</v>
-      </c>
-      <c r="C14" t="s">
-        <v>176</v>
       </c>
       <c r="D14" s="1">
         <v>45885.491481481484</v>
@@ -7196,18 +7200,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" t="s">
         <v>175</v>
-      </c>
-      <c r="C16" t="s">
-        <v>176</v>
       </c>
       <c r="D16" s="1">
         <v>45887.315196759257</v>
@@ -7216,15 +7220,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" t="s">
         <v>175</v>
-      </c>
-      <c r="C17" t="s">
-        <v>176</v>
       </c>
       <c r="D17" s="1">
         <v>45888.329733796294</v>
@@ -7233,15 +7237,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" t="s">
         <v>175</v>
-      </c>
-      <c r="C18" t="s">
-        <v>176</v>
       </c>
       <c r="D18" s="1">
         <v>45888.659467592595</v>
@@ -7250,15 +7254,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" t="s">
         <v>175</v>
-      </c>
-      <c r="C19" t="s">
-        <v>176</v>
       </c>
       <c r="D19" s="1">
         <v>45888.660671296297</v>
@@ -7267,15 +7271,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" t="s">
         <v>175</v>
-      </c>
-      <c r="C20" t="s">
-        <v>176</v>
       </c>
       <c r="D20" s="1">
         <v>45888.834548611114</v>
@@ -7284,15 +7288,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" t="s">
         <v>175</v>
-      </c>
-      <c r="C21" t="s">
-        <v>176</v>
       </c>
       <c r="D21" s="1">
         <v>45889.664756944447</v>

</xml_diff>